<commit_message>
word list updated hsk 1-4
</commit_message>
<xml_diff>
--- a/hsk-wordlist.xlsx
+++ b/hsk-wordlist.xlsx
@@ -5,27 +5,39 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\projects\flashcards\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\projects\hsk-flashcards\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{99E7D5D1-A2B7-4C8C-AA63-B3DEF317AF95}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B630ACC9-6200-4978-ACDB-DC24E54B6D13}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-90" yWindow="0" windowWidth="12980" windowHeight="15370" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="hsk1" sheetId="2" r:id="rId1"/>
+    <sheet name="hsk2" sheetId="3" r:id="rId2"/>
+    <sheet name="hsk3" sheetId="4" r:id="rId3"/>
+    <sheet name="hsk4" sheetId="1" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="620" uniqueCount="618">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1268" uniqueCount="1221">
   <si>
     <t>法律</t>
   </si>
@@ -1879,6 +1891,1815 @@
   </si>
   <si>
     <t>掉</t>
+  </si>
+  <si>
+    <t>你</t>
+  </si>
+  <si>
+    <t>好</t>
+  </si>
+  <si>
+    <t>您</t>
+  </si>
+  <si>
+    <t>你们</t>
+  </si>
+  <si>
+    <t>对不起</t>
+  </si>
+  <si>
+    <t>没关系</t>
+  </si>
+  <si>
+    <t>谢谢</t>
+  </si>
+  <si>
+    <t>不</t>
+  </si>
+  <si>
+    <t>不客气</t>
+  </si>
+  <si>
+    <t>再见</t>
+  </si>
+  <si>
+    <t>是</t>
+  </si>
+  <si>
+    <t>老师</t>
+  </si>
+  <si>
+    <t>吗</t>
+  </si>
+  <si>
+    <t>学生</t>
+  </si>
+  <si>
+    <t>人</t>
+  </si>
+  <si>
+    <t>叫</t>
+  </si>
+  <si>
+    <t>什么</t>
+  </si>
+  <si>
+    <t>名字</t>
+  </si>
+  <si>
+    <t>我</t>
+  </si>
+  <si>
+    <t>她</t>
+  </si>
+  <si>
+    <t>谁</t>
+  </si>
+  <si>
+    <t>的</t>
+  </si>
+  <si>
+    <t>汉语</t>
+  </si>
+  <si>
+    <t>哪</t>
+  </si>
+  <si>
+    <t>国</t>
+  </si>
+  <si>
+    <t>呢</t>
+  </si>
+  <si>
+    <t>他</t>
+  </si>
+  <si>
+    <t>同学</t>
+  </si>
+  <si>
+    <t>朋友</t>
+  </si>
+  <si>
+    <t>家</t>
+  </si>
+  <si>
+    <t>有</t>
+  </si>
+  <si>
+    <t>口</t>
+  </si>
+  <si>
+    <t>女儿</t>
+  </si>
+  <si>
+    <t>几</t>
+  </si>
+  <si>
+    <t>岁</t>
+  </si>
+  <si>
+    <t>了</t>
+  </si>
+  <si>
+    <t>今年</t>
+  </si>
+  <si>
+    <t>多</t>
+  </si>
+  <si>
+    <t>大</t>
+  </si>
+  <si>
+    <t>会</t>
+  </si>
+  <si>
+    <t>说</t>
+  </si>
+  <si>
+    <t>妈妈</t>
+  </si>
+  <si>
+    <t>菜</t>
+  </si>
+  <si>
+    <t>很</t>
+  </si>
+  <si>
+    <t>好吃</t>
+  </si>
+  <si>
+    <t>做</t>
+  </si>
+  <si>
+    <t>写</t>
+  </si>
+  <si>
+    <t>汉字</t>
+  </si>
+  <si>
+    <t>字</t>
+  </si>
+  <si>
+    <t>怎么</t>
+  </si>
+  <si>
+    <t>读</t>
+  </si>
+  <si>
+    <t>请</t>
+  </si>
+  <si>
+    <t>问</t>
+  </si>
+  <si>
+    <t>今天</t>
+  </si>
+  <si>
+    <t>号</t>
+  </si>
+  <si>
+    <t>月</t>
+  </si>
+  <si>
+    <t>星期</t>
+  </si>
+  <si>
+    <t>昨天</t>
+  </si>
+  <si>
+    <t>明天</t>
+  </si>
+  <si>
+    <t>去</t>
+  </si>
+  <si>
+    <t>学校</t>
+  </si>
+  <si>
+    <t>看</t>
+  </si>
+  <si>
+    <t>书</t>
+  </si>
+  <si>
+    <t>想</t>
+  </si>
+  <si>
+    <t>喝</t>
+  </si>
+  <si>
+    <t>茶</t>
+  </si>
+  <si>
+    <t>吃</t>
+  </si>
+  <si>
+    <t>米饭</t>
+  </si>
+  <si>
+    <t>买</t>
+  </si>
+  <si>
+    <t>个</t>
+  </si>
+  <si>
+    <t>下午</t>
+  </si>
+  <si>
+    <t>商店</t>
+  </si>
+  <si>
+    <t>杯子</t>
+  </si>
+  <si>
+    <t>这</t>
+  </si>
+  <si>
+    <t>多少</t>
+  </si>
+  <si>
+    <t>钱</t>
+  </si>
+  <si>
+    <t>快</t>
+  </si>
+  <si>
+    <t>那</t>
+  </si>
+  <si>
+    <t>小</t>
+  </si>
+  <si>
+    <t>猫</t>
+  </si>
+  <si>
+    <t>在</t>
+  </si>
+  <si>
+    <t>那人</t>
+  </si>
+  <si>
+    <t>狗</t>
+  </si>
+  <si>
+    <t>椅子</t>
+  </si>
+  <si>
+    <t>下面</t>
+  </si>
+  <si>
+    <t>哪人</t>
+  </si>
+  <si>
+    <t>儿子</t>
+  </si>
+  <si>
+    <t>医院</t>
+  </si>
+  <si>
+    <t>医生</t>
+  </si>
+  <si>
+    <t>工作</t>
+  </si>
+  <si>
+    <t>爸爸</t>
+  </si>
+  <si>
+    <t>桌子</t>
+  </si>
+  <si>
+    <t>上</t>
+  </si>
+  <si>
+    <t>电脑</t>
+  </si>
+  <si>
+    <t>和</t>
+  </si>
+  <si>
+    <t>本</t>
+  </si>
+  <si>
+    <t>里</t>
+  </si>
+  <si>
+    <t>前面</t>
+  </si>
+  <si>
+    <t>后面</t>
+  </si>
+  <si>
+    <t>这儿</t>
+  </si>
+  <si>
+    <t>没有</t>
+  </si>
+  <si>
+    <t>能</t>
+  </si>
+  <si>
+    <t>现在</t>
+  </si>
+  <si>
+    <t>点</t>
+  </si>
+  <si>
+    <t>分</t>
+  </si>
+  <si>
+    <t>中午</t>
+  </si>
+  <si>
+    <t>吃饭</t>
+  </si>
+  <si>
+    <t>时候</t>
+  </si>
+  <si>
+    <t>回</t>
+  </si>
+  <si>
+    <t>我们</t>
+  </si>
+  <si>
+    <t>电影</t>
+  </si>
+  <si>
+    <t>住</t>
+  </si>
+  <si>
+    <t>前</t>
+  </si>
+  <si>
+    <t>天气</t>
+  </si>
+  <si>
+    <t>怎么样</t>
+  </si>
+  <si>
+    <t>太</t>
+  </si>
+  <si>
+    <t>热</t>
+  </si>
+  <si>
+    <t>冷</t>
+  </si>
+  <si>
+    <t>下雨</t>
+  </si>
+  <si>
+    <t>小姐</t>
+  </si>
+  <si>
+    <t>来</t>
+  </si>
+  <si>
+    <t>身体</t>
+  </si>
+  <si>
+    <t>爱</t>
+  </si>
+  <si>
+    <t>些</t>
+  </si>
+  <si>
+    <t>水果</t>
+  </si>
+  <si>
+    <t>水</t>
+  </si>
+  <si>
+    <t>喂</t>
+  </si>
+  <si>
+    <t>也</t>
+  </si>
+  <si>
+    <t>学习</t>
+  </si>
+  <si>
+    <t>上午</t>
+  </si>
+  <si>
+    <t>睡觉</t>
+  </si>
+  <si>
+    <t>电视</t>
+  </si>
+  <si>
+    <t>喜欢</t>
+  </si>
+  <si>
+    <t>给</t>
+  </si>
+  <si>
+    <t>打电话</t>
+  </si>
+  <si>
+    <t>吧</t>
+  </si>
+  <si>
+    <t>东西</t>
+  </si>
+  <si>
+    <t>一点儿</t>
+  </si>
+  <si>
+    <t>苹果</t>
+  </si>
+  <si>
+    <t>看见</t>
+  </si>
+  <si>
+    <t>先生</t>
+  </si>
+  <si>
+    <t>开</t>
+  </si>
+  <si>
+    <t>车</t>
+  </si>
+  <si>
+    <t>回来</t>
+  </si>
+  <si>
+    <t>分钟</t>
+  </si>
+  <si>
+    <t>后</t>
+  </si>
+  <si>
+    <t>衣服</t>
+  </si>
+  <si>
+    <t>漂亮</t>
+  </si>
+  <si>
+    <t>啊</t>
+  </si>
+  <si>
+    <t>少</t>
+  </si>
+  <si>
+    <t>这些</t>
+  </si>
+  <si>
+    <t>都</t>
+  </si>
+  <si>
+    <t>认识</t>
+  </si>
+  <si>
+    <t>年</t>
+  </si>
+  <si>
+    <t>大学</t>
+  </si>
+  <si>
+    <t>饭店</t>
+  </si>
+  <si>
+    <t>出租车</t>
+  </si>
+  <si>
+    <t>一起</t>
+  </si>
+  <si>
+    <t>高兴</t>
+  </si>
+  <si>
+    <t>听</t>
+  </si>
+  <si>
+    <t>飞机</t>
+  </si>
+  <si>
+    <t>旅游</t>
+  </si>
+  <si>
+    <t>觉得</t>
+  </si>
+  <si>
+    <t>最</t>
+  </si>
+  <si>
+    <t>为什么</t>
+  </si>
+  <si>
+    <t>运动</t>
+  </si>
+  <si>
+    <t>踢足球</t>
+  </si>
+  <si>
+    <t>要</t>
+  </si>
+  <si>
+    <t>新</t>
+  </si>
+  <si>
+    <t>它</t>
+  </si>
+  <si>
+    <t>眼睛</t>
+  </si>
+  <si>
+    <t>生病</t>
+  </si>
+  <si>
+    <t>每</t>
+  </si>
+  <si>
+    <t>早上</t>
+  </si>
+  <si>
+    <t>跑步</t>
+  </si>
+  <si>
+    <t>起床</t>
+  </si>
+  <si>
+    <t>药</t>
+  </si>
+  <si>
+    <t>出院</t>
+  </si>
+  <si>
+    <t>高</t>
+  </si>
+  <si>
+    <t>米</t>
+  </si>
+  <si>
+    <t>知道</t>
+  </si>
+  <si>
+    <t>休息</t>
+  </si>
+  <si>
+    <t>忙</t>
+  </si>
+  <si>
+    <t>时间</t>
+  </si>
+  <si>
+    <t>手表</t>
+  </si>
+  <si>
+    <t>千</t>
+  </si>
+  <si>
+    <t>报纸</t>
+  </si>
+  <si>
+    <t>送</t>
+  </si>
+  <si>
+    <t>一下</t>
+  </si>
+  <si>
+    <t>牛奶</t>
+  </si>
+  <si>
+    <t>房间</t>
+  </si>
+  <si>
+    <t>丈夫</t>
+  </si>
+  <si>
+    <t>旁边</t>
+  </si>
+  <si>
+    <t>真</t>
+  </si>
+  <si>
+    <t>粉色</t>
+  </si>
+  <si>
+    <t>颜色</t>
+  </si>
+  <si>
+    <t>左边</t>
+  </si>
+  <si>
+    <t>红色</t>
+  </si>
+  <si>
+    <t>生日</t>
+  </si>
+  <si>
+    <t>快乐</t>
+  </si>
+  <si>
+    <t>接</t>
+  </si>
+  <si>
+    <t>晚上</t>
+  </si>
+  <si>
+    <t>非常</t>
+  </si>
+  <si>
+    <t>开始</t>
+  </si>
+  <si>
+    <t>已经</t>
+  </si>
+  <si>
+    <t>长</t>
+  </si>
+  <si>
+    <t>两</t>
+  </si>
+  <si>
+    <t>帮</t>
+  </si>
+  <si>
+    <t>介绍</t>
+  </si>
+  <si>
+    <t>外面</t>
+  </si>
+  <si>
+    <t>准备</t>
+  </si>
+  <si>
+    <t>就</t>
+  </si>
+  <si>
+    <t>鱼</t>
+  </si>
+  <si>
+    <t>件</t>
+  </si>
+  <si>
+    <t>还</t>
+  </si>
+  <si>
+    <t>可以</t>
+  </si>
+  <si>
+    <t>不错</t>
+  </si>
+  <si>
+    <t>考试</t>
+  </si>
+  <si>
+    <t>意思</t>
+  </si>
+  <si>
+    <t>咖啡</t>
+  </si>
+  <si>
+    <t>对</t>
+  </si>
+  <si>
+    <t>以后</t>
+  </si>
+  <si>
+    <t>门</t>
+  </si>
+  <si>
+    <t>外</t>
+  </si>
+  <si>
+    <t>自行车</t>
+  </si>
+  <si>
+    <t>羊肉</t>
+  </si>
+  <si>
+    <t>面条</t>
+  </si>
+  <si>
+    <t>打篮球</t>
+  </si>
+  <si>
+    <t>因为</t>
+  </si>
+  <si>
+    <t>所以</t>
+  </si>
+  <si>
+    <t>游泳</t>
+  </si>
+  <si>
+    <t>经常</t>
+  </si>
+  <si>
+    <t>公斤</t>
+  </si>
+  <si>
+    <t>姐姐</t>
+  </si>
+  <si>
+    <t>教室</t>
+  </si>
+  <si>
+    <t>机场</t>
+  </si>
+  <si>
+    <t>路</t>
+  </si>
+  <si>
+    <t>离</t>
+  </si>
+  <si>
+    <t>公司</t>
+  </si>
+  <si>
+    <t>远</t>
+  </si>
+  <si>
+    <t>公共汽车</t>
+  </si>
+  <si>
+    <t>小时</t>
+  </si>
+  <si>
+    <t>慢</t>
+  </si>
+  <si>
+    <t>过</t>
+  </si>
+  <si>
+    <t>走</t>
+  </si>
+  <si>
+    <t>到</t>
+  </si>
+  <si>
+    <t>再</t>
+  </si>
+  <si>
+    <t>让</t>
+  </si>
+  <si>
+    <t>告诉</t>
+  </si>
+  <si>
+    <t>找</t>
+  </si>
+  <si>
+    <t>事情</t>
+  </si>
+  <si>
+    <t>服务员</t>
+  </si>
+  <si>
+    <t>白</t>
+  </si>
+  <si>
+    <t>黑</t>
+  </si>
+  <si>
+    <t>贵</t>
+  </si>
+  <si>
+    <t>错</t>
+  </si>
+  <si>
+    <t>从</t>
+  </si>
+  <si>
+    <t>跳舞</t>
+  </si>
+  <si>
+    <t>第一</t>
+  </si>
+  <si>
+    <t>希望</t>
+  </si>
+  <si>
+    <t>问题</t>
+  </si>
+  <si>
+    <t>欢迎</t>
+  </si>
+  <si>
+    <t>上班</t>
+  </si>
+  <si>
+    <t>懂</t>
+  </si>
+  <si>
+    <t>完</t>
+  </si>
+  <si>
+    <t>题</t>
+  </si>
+  <si>
+    <t>课</t>
+  </si>
+  <si>
+    <t>帮助</t>
+  </si>
+  <si>
+    <t>别</t>
+  </si>
+  <si>
+    <t>哥哥</t>
+  </si>
+  <si>
+    <t>鸡蛋</t>
+  </si>
+  <si>
+    <t>西瓜</t>
+  </si>
+  <si>
+    <t>正在</t>
+  </si>
+  <si>
+    <t>手机</t>
+  </si>
+  <si>
+    <t>洗</t>
+  </si>
+  <si>
+    <t>唱歌</t>
+  </si>
+  <si>
+    <t>男</t>
+  </si>
+  <si>
+    <t>说话</t>
+  </si>
+  <si>
+    <t>可能</t>
+  </si>
+  <si>
+    <t>去年</t>
+  </si>
+  <si>
+    <t>姓</t>
+  </si>
+  <si>
+    <t>女</t>
+  </si>
+  <si>
+    <t>孩子</t>
+  </si>
+  <si>
+    <t>右边</t>
+  </si>
+  <si>
+    <t>比</t>
+  </si>
+  <si>
+    <t>便宜</t>
+  </si>
+  <si>
+    <t>妻子</t>
+  </si>
+  <si>
+    <t>雪</t>
+  </si>
+  <si>
+    <t>零</t>
+  </si>
+  <si>
+    <t>度</t>
+  </si>
+  <si>
+    <t>穿</t>
+  </si>
+  <si>
+    <t>进</t>
+  </si>
+  <si>
+    <t>弟弟</t>
+  </si>
+  <si>
+    <t>近</t>
+  </si>
+  <si>
+    <t>着</t>
+  </si>
+  <si>
+    <t>手</t>
+  </si>
+  <si>
+    <t>拿</t>
+  </si>
+  <si>
+    <t>铅笔</t>
+  </si>
+  <si>
+    <t>班</t>
+  </si>
+  <si>
+    <t>笑</t>
+  </si>
+  <si>
+    <t>冰棺</t>
+  </si>
+  <si>
+    <t>一直</t>
+  </si>
+  <si>
+    <t>往</t>
+  </si>
+  <si>
+    <t>路口</t>
+  </si>
+  <si>
+    <t>有意思</t>
+  </si>
+  <si>
+    <t>但是</t>
+  </si>
+  <si>
+    <t>虽然</t>
+  </si>
+  <si>
+    <t>次</t>
+  </si>
+  <si>
+    <t>玩儿</t>
+  </si>
+  <si>
+    <t>晴</t>
+  </si>
+  <si>
+    <t>百</t>
+  </si>
+  <si>
+    <t>日</t>
+  </si>
+  <si>
+    <t>新年</t>
+  </si>
+  <si>
+    <t>票</t>
+  </si>
+  <si>
+    <t>火车站</t>
+  </si>
+  <si>
+    <t>大家</t>
+  </si>
+  <si>
+    <t>更</t>
+  </si>
+  <si>
+    <t>妹妹</t>
+  </si>
+  <si>
+    <t>阴</t>
+  </si>
+  <si>
+    <t>周末</t>
+  </si>
+  <si>
+    <t>打算</t>
+  </si>
+  <si>
+    <t>跟</t>
+  </si>
+  <si>
+    <t>游戏</t>
+  </si>
+  <si>
+    <t>作业</t>
+  </si>
+  <si>
+    <t>着急</t>
+  </si>
+  <si>
+    <t>复习</t>
+  </si>
+  <si>
+    <t>南方</t>
+  </si>
+  <si>
+    <t>北方</t>
+  </si>
+  <si>
+    <t>面包</t>
+  </si>
+  <si>
+    <t>带</t>
+  </si>
+  <si>
+    <t>地图</t>
+  </si>
+  <si>
+    <t>搬</t>
+  </si>
+  <si>
+    <t>腿</t>
+  </si>
+  <si>
+    <t>疼</t>
+  </si>
+  <si>
+    <t>脚</t>
+  </si>
+  <si>
+    <t>树</t>
+  </si>
+  <si>
+    <t>容易</t>
+  </si>
+  <si>
+    <t>难</t>
+  </si>
+  <si>
+    <t>太太</t>
+  </si>
+  <si>
+    <t>秘书</t>
+  </si>
+  <si>
+    <t>办公室</t>
+  </si>
+  <si>
+    <t>辆</t>
+  </si>
+  <si>
+    <t>楼</t>
+  </si>
+  <si>
+    <t>把</t>
+  </si>
+  <si>
+    <t>伞</t>
+  </si>
+  <si>
+    <t>胖</t>
+  </si>
+  <si>
+    <t>其实</t>
+  </si>
+  <si>
+    <t>瘦</t>
+  </si>
+  <si>
+    <t>还是</t>
+  </si>
+  <si>
+    <t>爬山</t>
+  </si>
+  <si>
+    <t>小心</t>
+  </si>
+  <si>
+    <t>条</t>
+  </si>
+  <si>
+    <t>裤子</t>
+  </si>
+  <si>
+    <t>记得</t>
+  </si>
+  <si>
+    <t>衬衫</t>
+  </si>
+  <si>
+    <t>元</t>
+  </si>
+  <si>
+    <t>新鲜</t>
+  </si>
+  <si>
+    <t>甜</t>
+  </si>
+  <si>
+    <t>只</t>
+  </si>
+  <si>
+    <t>放</t>
+  </si>
+  <si>
+    <t>饮料</t>
+  </si>
+  <si>
+    <t>或者</t>
+  </si>
+  <si>
+    <t>舒服</t>
+  </si>
+  <si>
+    <t>花</t>
+  </si>
+  <si>
+    <t>绿</t>
+  </si>
+  <si>
+    <t>比赛</t>
+  </si>
+  <si>
+    <t>照片</t>
+  </si>
+  <si>
+    <t>年级</t>
+  </si>
+  <si>
+    <t>又</t>
+  </si>
+  <si>
+    <t>聪明</t>
+  </si>
+  <si>
+    <t>热情</t>
+  </si>
+  <si>
+    <t>努力</t>
+  </si>
+  <si>
+    <t>总是</t>
+  </si>
+  <si>
+    <t>回答</t>
+  </si>
+  <si>
+    <t>站</t>
+  </si>
+  <si>
+    <t>饿</t>
+  </si>
+  <si>
+    <t>超市</t>
+  </si>
+  <si>
+    <t>蛋糕</t>
+  </si>
+  <si>
+    <t>年轻</t>
+  </si>
+  <si>
+    <t>认真</t>
+  </si>
+  <si>
+    <t>客人</t>
+  </si>
+  <si>
+    <t>发烧</t>
+  </si>
+  <si>
+    <t>为</t>
+  </si>
+  <si>
+    <t>照顾</t>
+  </si>
+  <si>
+    <t>用</t>
+  </si>
+  <si>
+    <t>感冒</t>
+  </si>
+  <si>
+    <t>张</t>
+  </si>
+  <si>
+    <t>季节</t>
+  </si>
+  <si>
+    <t>当然</t>
+  </si>
+  <si>
+    <t>春天</t>
+  </si>
+  <si>
+    <t>草</t>
+  </si>
+  <si>
+    <t>夏天</t>
+  </si>
+  <si>
+    <t>裙子</t>
+  </si>
+  <si>
+    <t>最近</t>
+  </si>
+  <si>
+    <t>越</t>
+  </si>
+  <si>
+    <t>突然</t>
+  </si>
+  <si>
+    <t>离开</t>
+  </si>
+  <si>
+    <t>清楚</t>
+  </si>
+  <si>
+    <t>刚才</t>
+  </si>
+  <si>
+    <t>帮忙</t>
+  </si>
+  <si>
+    <t>特别</t>
+  </si>
+  <si>
+    <t>讲</t>
+  </si>
+  <si>
+    <t>明白</t>
+  </si>
+  <si>
+    <t>锻炼</t>
+  </si>
+  <si>
+    <t>音乐</t>
+  </si>
+  <si>
+    <t>公园</t>
+  </si>
+  <si>
+    <t>聊天儿</t>
+  </si>
+  <si>
+    <t>睡着</t>
+  </si>
+  <si>
+    <t>同事</t>
+  </si>
+  <si>
+    <t>以前</t>
+  </si>
+  <si>
+    <t>银行</t>
+  </si>
+  <si>
+    <t>久</t>
+  </si>
+  <si>
+    <t>感兴趣</t>
+  </si>
+  <si>
+    <t>结婚</t>
+  </si>
+  <si>
+    <t>迟到</t>
+  </si>
+  <si>
+    <t>半</t>
+  </si>
+  <si>
+    <t>刻</t>
+  </si>
+  <si>
+    <t>差</t>
+  </si>
+  <si>
+    <t>满意</t>
+  </si>
+  <si>
+    <t>电梯</t>
+  </si>
+  <si>
+    <t>层</t>
+  </si>
+  <si>
+    <t>害怕</t>
+  </si>
+  <si>
+    <t>熊猫</t>
+  </si>
+  <si>
+    <t>见面</t>
+  </si>
+  <si>
+    <t>安静</t>
+  </si>
+  <si>
+    <t>可乐</t>
+  </si>
+  <si>
+    <t>一会儿</t>
+  </si>
+  <si>
+    <t>马上</t>
+  </si>
+  <si>
+    <t>洗手间</t>
+  </si>
+  <si>
+    <t>老</t>
+  </si>
+  <si>
+    <t>几乎</t>
+  </si>
+  <si>
+    <t>变化</t>
+  </si>
+  <si>
+    <t>健康</t>
+  </si>
+  <si>
+    <t>重要</t>
+  </si>
+  <si>
+    <t>中文</t>
+  </si>
+  <si>
+    <t>一样</t>
+  </si>
+  <si>
+    <t>最后</t>
+  </si>
+  <si>
+    <t>放心</t>
+  </si>
+  <si>
+    <t>一定</t>
+  </si>
+  <si>
+    <t>担心</t>
+  </si>
+  <si>
+    <t>比较</t>
+  </si>
+  <si>
+    <t>了解</t>
+  </si>
+  <si>
+    <t>先</t>
+  </si>
+  <si>
+    <t>中间</t>
+  </si>
+  <si>
+    <t>参加</t>
+  </si>
+  <si>
+    <t>影响</t>
+  </si>
+  <si>
+    <t>个子</t>
+  </si>
+  <si>
+    <t>矮</t>
+  </si>
+  <si>
+    <t>历史</t>
+  </si>
+  <si>
+    <t>体育</t>
+  </si>
+  <si>
+    <t>数学</t>
+  </si>
+  <si>
+    <t>方便</t>
+  </si>
+  <si>
+    <t>骑</t>
+  </si>
+  <si>
+    <t>旧</t>
+  </si>
+  <si>
+    <t>换</t>
+  </si>
+  <si>
+    <t>地方</t>
+  </si>
+  <si>
+    <t>中介</t>
+  </si>
+  <si>
+    <t>主要</t>
+  </si>
+  <si>
+    <t>环境</t>
+  </si>
+  <si>
+    <t>附近</t>
+  </si>
+  <si>
+    <t>图书馆</t>
+  </si>
+  <si>
+    <t>借</t>
+  </si>
+  <si>
+    <t>词典</t>
+  </si>
+  <si>
+    <t>灯</t>
+  </si>
+  <si>
+    <t>会议</t>
+  </si>
+  <si>
+    <t>结束</t>
+  </si>
+  <si>
+    <t>忘记</t>
+  </si>
+  <si>
+    <t>空调</t>
+  </si>
+  <si>
+    <t>关</t>
+  </si>
+  <si>
+    <t>地铁</t>
+  </si>
+  <si>
+    <t>双</t>
+  </si>
+  <si>
+    <t>筷子</t>
+  </si>
+  <si>
+    <t>啤酒</t>
+  </si>
+  <si>
+    <t>瓶子</t>
+  </si>
+  <si>
+    <t>笔记本</t>
+  </si>
+  <si>
+    <t>电子邮件</t>
+  </si>
+  <si>
+    <t>习惯</t>
+  </si>
+  <si>
+    <t>太阳</t>
+  </si>
+  <si>
+    <t>生气</t>
+  </si>
+  <si>
+    <t>行李箱</t>
+  </si>
+  <si>
+    <t>自己</t>
+  </si>
+  <si>
+    <t>包</t>
+  </si>
+  <si>
+    <t>发现</t>
+  </si>
+  <si>
+    <t>护照</t>
+  </si>
+  <si>
+    <t>起飞</t>
+  </si>
+  <si>
+    <t>司机</t>
+  </si>
+  <si>
+    <t>教</t>
+  </si>
+  <si>
+    <t>画</t>
+  </si>
+  <si>
+    <t>需要</t>
+  </si>
+  <si>
+    <t>黑板</t>
+  </si>
+  <si>
+    <t>终于</t>
+  </si>
+  <si>
+    <t>爷爷</t>
+  </si>
+  <si>
+    <t>礼物</t>
+  </si>
+  <si>
+    <t>奶奶</t>
+  </si>
+  <si>
+    <t>遇到</t>
+  </si>
+  <si>
+    <t>一边</t>
+  </si>
+  <si>
+    <t>过去</t>
+  </si>
+  <si>
+    <t>一般</t>
+  </si>
+  <si>
+    <t>愿意</t>
+  </si>
+  <si>
+    <t>起来</t>
+  </si>
+  <si>
+    <t>应该</t>
+  </si>
+  <si>
+    <t>校长</t>
+  </si>
+  <si>
+    <t>坏</t>
+  </si>
+  <si>
+    <t>打扫</t>
+  </si>
+  <si>
+    <t>干净</t>
+  </si>
+  <si>
+    <t>然后</t>
+  </si>
+  <si>
+    <t>冰箱</t>
+  </si>
+  <si>
+    <t>洗澡</t>
+  </si>
+  <si>
+    <t>节目</t>
+  </si>
+  <si>
+    <t>月亮</t>
+  </si>
+  <si>
+    <t>盘子</t>
+  </si>
+  <si>
+    <t>刮风</t>
+  </si>
+  <si>
+    <t>叔叔</t>
+  </si>
+  <si>
+    <t>阿姨</t>
+  </si>
+  <si>
+    <t>故事</t>
+  </si>
+  <si>
+    <t>声音</t>
+  </si>
+  <si>
+    <t>菜单</t>
+  </si>
+  <si>
+    <t>简单</t>
+  </si>
+  <si>
+    <t>香蕉</t>
+  </si>
+  <si>
+    <t>留学</t>
+  </si>
+  <si>
+    <t>水平</t>
+  </si>
+  <si>
+    <t>提高</t>
+  </si>
+  <si>
+    <t>练习</t>
+  </si>
+  <si>
+    <t>完成</t>
+  </si>
+  <si>
+    <t>句子</t>
+  </si>
+  <si>
+    <t>其他</t>
+  </si>
+  <si>
+    <t>发</t>
+  </si>
+  <si>
+    <t>要求</t>
+  </si>
+  <si>
+    <t>除了</t>
+  </si>
+  <si>
+    <t>新闻</t>
+  </si>
+  <si>
+    <t>极了</t>
+  </si>
+  <si>
+    <t>节日</t>
+  </si>
+  <si>
+    <t>世界</t>
+  </si>
+  <si>
+    <t>街道</t>
+  </si>
+  <si>
+    <t>上网</t>
+  </si>
+  <si>
+    <t>文化</t>
+  </si>
+  <si>
+    <t>城市</t>
+  </si>
+  <si>
+    <t>如果</t>
+  </si>
+  <si>
+    <t>认为</t>
+  </si>
+  <si>
+    <t>皮鞋</t>
+  </si>
+  <si>
+    <t>帽子</t>
+  </si>
+  <si>
+    <t>可爱</t>
+  </si>
+  <si>
+    <t>鼻子</t>
+  </si>
+  <si>
+    <t>头发</t>
+  </si>
+  <si>
+    <t>检查</t>
+  </si>
+  <si>
+    <t>刷牙</t>
+  </si>
+  <si>
+    <t>关系</t>
+  </si>
+  <si>
+    <t>别人</t>
+  </si>
+  <si>
+    <t>请假</t>
+  </si>
+  <si>
+    <t>一共</t>
+  </si>
+  <si>
+    <t>邻居</t>
+  </si>
+  <si>
+    <t>后来</t>
+  </si>
+  <si>
+    <t>爱好</t>
+  </si>
+  <si>
+    <t>办法</t>
+  </si>
+  <si>
+    <t>饱</t>
+  </si>
+  <si>
+    <t>为了</t>
+  </si>
+  <si>
+    <t>决定</t>
+  </si>
+  <si>
+    <t>选择</t>
+  </si>
+  <si>
+    <t>冬天</t>
+  </si>
+  <si>
+    <t>必须</t>
+  </si>
+  <si>
+    <t>根据</t>
+  </si>
+  <si>
+    <t>渴</t>
+  </si>
+  <si>
+    <t>向</t>
+  </si>
+  <si>
+    <t>万</t>
+  </si>
+  <si>
+    <t>嘴</t>
+  </si>
+  <si>
+    <t>动物</t>
+  </si>
+  <si>
+    <t>段</t>
+  </si>
+  <si>
+    <t>不但</t>
+  </si>
+  <si>
+    <t>而且</t>
+  </si>
+  <si>
+    <t>有名</t>
+  </si>
+  <si>
+    <t>同意</t>
+  </si>
+  <si>
+    <t>相信</t>
+  </si>
+  <si>
+    <t>关于</t>
+  </si>
+  <si>
+    <t>机会</t>
+  </si>
+  <si>
+    <t>国家</t>
+  </si>
+  <si>
+    <t>种</t>
+  </si>
+  <si>
+    <t>奇怪</t>
+  </si>
+  <si>
+    <t>地</t>
+  </si>
+  <si>
+    <t>耳朵</t>
+  </si>
+  <si>
+    <t>脸</t>
+  </si>
+  <si>
+    <t>短</t>
+  </si>
+  <si>
+    <t>马</t>
+  </si>
+  <si>
+    <t>位</t>
+  </si>
+  <si>
+    <t>蓝</t>
+  </si>
+  <si>
+    <t>秋天</t>
+  </si>
+  <si>
+    <t>鸟</t>
+  </si>
+  <si>
+    <t>哭</t>
+  </si>
+  <si>
+    <t>黄河</t>
+  </si>
+  <si>
+    <t>船</t>
+  </si>
+  <si>
+    <t>经过</t>
+  </si>
+  <si>
+    <t>照相机</t>
+  </si>
+  <si>
+    <t>被</t>
+  </si>
+  <si>
+    <t>难过</t>
+  </si>
+  <si>
+    <t>东</t>
+  </si>
+  <si>
+    <t>信用卡</t>
+  </si>
+  <si>
+    <t>关心</t>
+  </si>
+  <si>
+    <t>只有</t>
+  </si>
+  <si>
+    <t>才</t>
+  </si>
+  <si>
+    <t>成绩</t>
+  </si>
+  <si>
+    <t>碗</t>
+  </si>
+  <si>
+    <t>解决</t>
+  </si>
+  <si>
+    <t>试</t>
+  </si>
+  <si>
+    <t>多么</t>
   </si>
 </sst>
 </file>
@@ -2195,10 +4016,2104 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{51947C01-8969-4A30-B1EB-A0D512A7B015}">
+  <dimension ref="A1:O16"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A7" sqref="A7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetData>
+    <row r="1" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
+        <v>618</v>
+      </c>
+      <c r="B1" t="s">
+        <v>624</v>
+      </c>
+      <c r="C1" t="s">
+        <v>633</v>
+      </c>
+      <c r="D1" t="s">
+        <v>637</v>
+      </c>
+      <c r="E1" t="s">
+        <v>647</v>
+      </c>
+      <c r="F1" t="s">
+        <v>657</v>
+      </c>
+      <c r="G1" t="s">
+        <v>669</v>
+      </c>
+      <c r="H1" t="s">
+        <v>681</v>
+      </c>
+      <c r="I1" t="s">
+        <v>696</v>
+      </c>
+      <c r="J1" t="s">
+        <v>709</v>
+      </c>
+      <c r="K1" t="s">
+        <v>720</v>
+      </c>
+      <c r="L1" t="s">
+        <v>731</v>
+      </c>
+      <c r="M1" t="s">
+        <v>744</v>
+      </c>
+      <c r="N1" t="s">
+        <v>754</v>
+      </c>
+      <c r="O1" t="s">
+        <v>770</v>
+      </c>
+    </row>
+    <row r="2" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>619</v>
+      </c>
+      <c r="B2" t="s">
+        <v>625</v>
+      </c>
+      <c r="C2" t="s">
+        <v>634</v>
+      </c>
+      <c r="D2" t="s">
+        <v>638</v>
+      </c>
+      <c r="E2" t="s">
+        <v>648</v>
+      </c>
+      <c r="F2" t="s">
+        <v>658</v>
+      </c>
+      <c r="G2" t="s">
+        <v>670</v>
+      </c>
+      <c r="H2" t="s">
+        <v>682</v>
+      </c>
+      <c r="I2" t="s">
+        <v>697</v>
+      </c>
+      <c r="J2" t="s">
+        <v>710</v>
+      </c>
+      <c r="K2" t="s">
+        <v>721</v>
+      </c>
+      <c r="L2" t="s">
+        <v>732</v>
+      </c>
+      <c r="M2" t="s">
+        <v>745</v>
+      </c>
+      <c r="N2" t="s">
+        <v>755</v>
+      </c>
+      <c r="O2" t="s">
+        <v>771</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>620</v>
+      </c>
+      <c r="B3" t="s">
+        <v>626</v>
+      </c>
+      <c r="C3" t="s">
+        <v>635</v>
+      </c>
+      <c r="D3" t="s">
+        <v>639</v>
+      </c>
+      <c r="E3" t="s">
+        <v>649</v>
+      </c>
+      <c r="F3" t="s">
+        <v>659</v>
+      </c>
+      <c r="G3" t="s">
+        <v>671</v>
+      </c>
+      <c r="H3" t="s">
+        <v>683</v>
+      </c>
+      <c r="I3" t="s">
+        <v>698</v>
+      </c>
+      <c r="J3" t="s">
+        <v>711</v>
+      </c>
+      <c r="K3" t="s">
+        <v>722</v>
+      </c>
+      <c r="L3" t="s">
+        <v>733</v>
+      </c>
+      <c r="M3" t="s">
+        <v>746</v>
+      </c>
+      <c r="N3" t="s">
+        <v>756</v>
+      </c>
+      <c r="O3" t="s">
+        <v>772</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>621</v>
+      </c>
+      <c r="B4" t="s">
+        <v>627</v>
+      </c>
+      <c r="C4" t="s">
+        <v>636</v>
+      </c>
+      <c r="D4" t="s">
+        <v>640</v>
+      </c>
+      <c r="E4" t="s">
+        <v>650</v>
+      </c>
+      <c r="F4" t="s">
+        <v>660</v>
+      </c>
+      <c r="G4" t="s">
+        <v>672</v>
+      </c>
+      <c r="H4" t="s">
+        <v>684</v>
+      </c>
+      <c r="I4" t="s">
+        <v>699</v>
+      </c>
+      <c r="J4" t="s">
+        <v>712</v>
+      </c>
+      <c r="K4" t="s">
+        <v>723</v>
+      </c>
+      <c r="L4" t="s">
+        <v>734</v>
+      </c>
+      <c r="M4" t="s">
+        <v>747</v>
+      </c>
+      <c r="N4" t="s">
+        <v>757</v>
+      </c>
+      <c r="O4" t="s">
+        <v>773</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>622</v>
+      </c>
+      <c r="C5" t="s">
+        <v>628</v>
+      </c>
+      <c r="D5" t="s">
+        <v>641</v>
+      </c>
+      <c r="E5" t="s">
+        <v>651</v>
+      </c>
+      <c r="F5" t="s">
+        <v>661</v>
+      </c>
+      <c r="G5" t="s">
+        <v>673</v>
+      </c>
+      <c r="H5" t="s">
+        <v>685</v>
+      </c>
+      <c r="I5" t="s">
+        <v>700</v>
+      </c>
+      <c r="J5" t="s">
+        <v>713</v>
+      </c>
+      <c r="K5" t="s">
+        <v>724</v>
+      </c>
+      <c r="L5" t="s">
+        <v>735</v>
+      </c>
+      <c r="M5" t="s">
+        <v>748</v>
+      </c>
+      <c r="N5" t="s">
+        <v>758</v>
+      </c>
+      <c r="O5" t="s">
+        <v>774</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
+        <v>623</v>
+      </c>
+      <c r="C6" t="s">
+        <v>629</v>
+      </c>
+      <c r="D6" t="s">
+        <v>642</v>
+      </c>
+      <c r="E6" t="s">
+        <v>652</v>
+      </c>
+      <c r="F6" t="s">
+        <v>662</v>
+      </c>
+      <c r="G6" t="s">
+        <v>674</v>
+      </c>
+      <c r="H6" t="s">
+        <v>688</v>
+      </c>
+      <c r="I6" t="s">
+        <v>701</v>
+      </c>
+      <c r="J6" t="s">
+        <v>714</v>
+      </c>
+      <c r="K6" t="s">
+        <v>725</v>
+      </c>
+      <c r="L6" t="s">
+        <v>736</v>
+      </c>
+      <c r="M6" t="s">
+        <v>749</v>
+      </c>
+      <c r="N6" t="s">
+        <v>759</v>
+      </c>
+      <c r="O6" t="s">
+        <v>775</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="C7" t="s">
+        <v>630</v>
+      </c>
+      <c r="D7" t="s">
+        <v>643</v>
+      </c>
+      <c r="E7" t="s">
+        <v>653</v>
+      </c>
+      <c r="F7" t="s">
+        <v>663</v>
+      </c>
+      <c r="G7" t="s">
+        <v>675</v>
+      </c>
+      <c r="H7" t="s">
+        <v>689</v>
+      </c>
+      <c r="I7" t="s">
+        <v>702</v>
+      </c>
+      <c r="J7" t="s">
+        <v>715</v>
+      </c>
+      <c r="K7" t="s">
+        <v>726</v>
+      </c>
+      <c r="L7" t="s">
+        <v>737</v>
+      </c>
+      <c r="M7" t="s">
+        <v>750</v>
+      </c>
+      <c r="N7" t="s">
+        <v>760</v>
+      </c>
+      <c r="O7" t="s">
+        <v>776</v>
+      </c>
+    </row>
+    <row r="8" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="C8" t="s">
+        <v>631</v>
+      </c>
+      <c r="D8" t="s">
+        <v>644</v>
+      </c>
+      <c r="E8" t="s">
+        <v>654</v>
+      </c>
+      <c r="F8" t="s">
+        <v>664</v>
+      </c>
+      <c r="G8" t="s">
+        <v>676</v>
+      </c>
+      <c r="H8" t="s">
+        <v>686</v>
+      </c>
+      <c r="I8" t="s">
+        <v>698</v>
+      </c>
+      <c r="J8" t="s">
+        <v>716</v>
+      </c>
+      <c r="K8" t="s">
+        <v>727</v>
+      </c>
+      <c r="L8" t="s">
+        <v>738</v>
+      </c>
+      <c r="M8" t="s">
+        <v>751</v>
+      </c>
+      <c r="N8" t="s">
+        <v>761</v>
+      </c>
+      <c r="O8" t="s">
+        <v>777</v>
+      </c>
+    </row>
+    <row r="9" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="C9" t="s">
+        <v>632</v>
+      </c>
+      <c r="D9" t="s">
+        <v>645</v>
+      </c>
+      <c r="E9" t="s">
+        <v>655</v>
+      </c>
+      <c r="F9" t="s">
+        <v>665</v>
+      </c>
+      <c r="G9" t="s">
+        <v>677</v>
+      </c>
+      <c r="H9" t="s">
+        <v>687</v>
+      </c>
+      <c r="I9" t="s">
+        <v>703</v>
+      </c>
+      <c r="J9" t="s">
+        <v>717</v>
+      </c>
+      <c r="K9" t="s">
+        <v>728</v>
+      </c>
+      <c r="L9" t="s">
+        <v>739</v>
+      </c>
+      <c r="M9" t="s">
+        <v>752</v>
+      </c>
+      <c r="N9" t="s">
+        <v>762</v>
+      </c>
+      <c r="O9" t="s">
+        <v>778</v>
+      </c>
+    </row>
+    <row r="10" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="D10" t="s">
+        <v>646</v>
+      </c>
+      <c r="E10" t="s">
+        <v>656</v>
+      </c>
+      <c r="F10" t="s">
+        <v>666</v>
+      </c>
+      <c r="G10" t="s">
+        <v>678</v>
+      </c>
+      <c r="H10" t="s">
+        <v>690</v>
+      </c>
+      <c r="I10" t="s">
+        <v>707</v>
+      </c>
+      <c r="J10" t="s">
+        <v>718</v>
+      </c>
+      <c r="K10" t="s">
+        <v>729</v>
+      </c>
+      <c r="L10" t="s">
+        <v>740</v>
+      </c>
+      <c r="M10" t="s">
+        <v>753</v>
+      </c>
+      <c r="N10" t="s">
+        <v>763</v>
+      </c>
+    </row>
+    <row r="11" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="F11" t="s">
+        <v>667</v>
+      </c>
+      <c r="G11" t="s">
+        <v>679</v>
+      </c>
+      <c r="H11" t="s">
+        <v>691</v>
+      </c>
+      <c r="I11" t="s">
+        <v>704</v>
+      </c>
+      <c r="J11" t="s">
+        <v>719</v>
+      </c>
+      <c r="K11" t="s">
+        <v>730</v>
+      </c>
+      <c r="L11" t="s">
+        <v>741</v>
+      </c>
+      <c r="N11" t="s">
+        <v>764</v>
+      </c>
+    </row>
+    <row r="12" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="F12" t="s">
+        <v>668</v>
+      </c>
+      <c r="G12" t="s">
+        <v>680</v>
+      </c>
+      <c r="H12" t="s">
+        <v>692</v>
+      </c>
+      <c r="I12" t="s">
+        <v>705</v>
+      </c>
+      <c r="J12" t="s">
+        <v>277</v>
+      </c>
+      <c r="L12" t="s">
+        <v>742</v>
+      </c>
+      <c r="N12" t="s">
+        <v>765</v>
+      </c>
+    </row>
+    <row r="13" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="H13" t="s">
+        <v>693</v>
+      </c>
+      <c r="I13" t="s">
+        <v>706</v>
+      </c>
+      <c r="L13" t="s">
+        <v>743</v>
+      </c>
+      <c r="N13" t="s">
+        <v>766</v>
+      </c>
+    </row>
+    <row r="14" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="H14" t="s">
+        <v>694</v>
+      </c>
+      <c r="I14" t="s">
+        <v>708</v>
+      </c>
+      <c r="N14" t="s">
+        <v>767</v>
+      </c>
+    </row>
+    <row r="15" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="H15" t="s">
+        <v>695</v>
+      </c>
+      <c r="N15" t="s">
+        <v>768</v>
+      </c>
+    </row>
+    <row r="16" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="N16" t="s">
+        <v>769</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{55641C87-CC01-401F-B2EC-F05E5CC7CADA}">
+  <dimension ref="A1:O14"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="O1" sqref="O1:O8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetData>
+    <row r="1" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
+        <v>779</v>
+      </c>
+      <c r="B1" t="s">
+        <v>789</v>
+      </c>
+      <c r="C1" t="s">
+        <v>802</v>
+      </c>
+      <c r="D1" t="s">
+        <v>816</v>
+      </c>
+      <c r="E1" t="s">
+        <v>827</v>
+      </c>
+      <c r="F1" t="s">
+        <v>840</v>
+      </c>
+      <c r="G1" t="s">
+        <v>852</v>
+      </c>
+      <c r="H1" t="s">
+        <v>864</v>
+      </c>
+      <c r="I1" t="s">
+        <v>873</v>
+      </c>
+      <c r="J1" t="s">
+        <v>884</v>
+      </c>
+      <c r="K1" t="s">
+        <v>893</v>
+      </c>
+      <c r="L1" t="s">
+        <v>48</v>
+      </c>
+      <c r="M1" t="s">
+        <v>912</v>
+      </c>
+      <c r="N1" t="s">
+        <v>922</v>
+      </c>
+      <c r="O1" t="s">
+        <v>929</v>
+      </c>
+    </row>
+    <row r="2" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>780</v>
+      </c>
+      <c r="B2" t="s">
+        <v>790</v>
+      </c>
+      <c r="C2" t="s">
+        <v>803</v>
+      </c>
+      <c r="D2" t="s">
+        <v>817</v>
+      </c>
+      <c r="E2" t="s">
+        <v>828</v>
+      </c>
+      <c r="F2" t="s">
+        <v>841</v>
+      </c>
+      <c r="G2" t="s">
+        <v>853</v>
+      </c>
+      <c r="H2" t="s">
+        <v>865</v>
+      </c>
+      <c r="I2" t="s">
+        <v>874</v>
+      </c>
+      <c r="J2" t="s">
+        <v>885</v>
+      </c>
+      <c r="K2" t="s">
+        <v>894</v>
+      </c>
+      <c r="L2" t="s">
+        <v>904</v>
+      </c>
+      <c r="M2" t="s">
+        <v>913</v>
+      </c>
+      <c r="N2" t="s">
+        <v>923</v>
+      </c>
+      <c r="O2" t="s">
+        <v>930</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>781</v>
+      </c>
+      <c r="B3" t="s">
+        <v>791</v>
+      </c>
+      <c r="C3" t="s">
+        <v>804</v>
+      </c>
+      <c r="D3" t="s">
+        <v>751</v>
+      </c>
+      <c r="E3" t="s">
+        <v>829</v>
+      </c>
+      <c r="F3" t="s">
+        <v>842</v>
+      </c>
+      <c r="G3" t="s">
+        <v>854</v>
+      </c>
+      <c r="H3" t="s">
+        <v>866</v>
+      </c>
+      <c r="I3" t="s">
+        <v>875</v>
+      </c>
+      <c r="J3" t="s">
+        <v>886</v>
+      </c>
+      <c r="K3" t="s">
+        <v>899</v>
+      </c>
+      <c r="L3" t="s">
+        <v>905</v>
+      </c>
+      <c r="M3" t="s">
+        <v>914</v>
+      </c>
+      <c r="N3" t="s">
+        <v>924</v>
+      </c>
+      <c r="O3" t="s">
+        <v>931</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>782</v>
+      </c>
+      <c r="B4" t="s">
+        <v>792</v>
+      </c>
+      <c r="C4" t="s">
+        <v>805</v>
+      </c>
+      <c r="D4" t="s">
+        <v>818</v>
+      </c>
+      <c r="E4" t="s">
+        <v>830</v>
+      </c>
+      <c r="F4" t="s">
+        <v>843</v>
+      </c>
+      <c r="G4" t="s">
+        <v>855</v>
+      </c>
+      <c r="H4" t="s">
+        <v>469</v>
+      </c>
+      <c r="I4" t="s">
+        <v>876</v>
+      </c>
+      <c r="J4" t="s">
+        <v>887</v>
+      </c>
+      <c r="K4" t="s">
+        <v>900</v>
+      </c>
+      <c r="L4" t="s">
+        <v>906</v>
+      </c>
+      <c r="M4" t="s">
+        <v>915</v>
+      </c>
+      <c r="N4" t="s">
+        <v>925</v>
+      </c>
+      <c r="O4" t="s">
+        <v>932</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>745</v>
+      </c>
+      <c r="B5" t="s">
+        <v>793</v>
+      </c>
+      <c r="C5" t="s">
+        <v>806</v>
+      </c>
+      <c r="D5" t="s">
+        <v>819</v>
+      </c>
+      <c r="E5" t="s">
+        <v>753</v>
+      </c>
+      <c r="F5" t="s">
+        <v>662</v>
+      </c>
+      <c r="G5" t="s">
+        <v>856</v>
+      </c>
+      <c r="H5" t="s">
+        <v>867</v>
+      </c>
+      <c r="I5" t="s">
+        <v>877</v>
+      </c>
+      <c r="J5" t="s">
+        <v>888</v>
+      </c>
+      <c r="K5" t="s">
+        <v>901</v>
+      </c>
+      <c r="L5" t="s">
+        <v>907</v>
+      </c>
+      <c r="M5" t="s">
+        <v>916</v>
+      </c>
+      <c r="N5" t="s">
+        <v>926</v>
+      </c>
+      <c r="O5" t="s">
+        <v>933</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
+        <v>783</v>
+      </c>
+      <c r="B6" t="s">
+        <v>794</v>
+      </c>
+      <c r="C6" t="s">
+        <v>807</v>
+      </c>
+      <c r="D6" t="s">
+        <v>670</v>
+      </c>
+      <c r="E6" t="s">
+        <v>831</v>
+      </c>
+      <c r="F6" t="s">
+        <v>844</v>
+      </c>
+      <c r="G6" t="s">
+        <v>857</v>
+      </c>
+      <c r="H6" t="s">
+        <v>868</v>
+      </c>
+      <c r="I6" t="s">
+        <v>878</v>
+      </c>
+      <c r="J6" t="s">
+        <v>889</v>
+      </c>
+      <c r="K6" t="s">
+        <v>902</v>
+      </c>
+      <c r="L6" t="s">
+        <v>908</v>
+      </c>
+      <c r="M6" t="s">
+        <v>823</v>
+      </c>
+      <c r="N6" t="s">
+        <v>927</v>
+      </c>
+      <c r="O6" t="s">
+        <v>934</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A7" t="s">
+        <v>784</v>
+      </c>
+      <c r="B7" t="s">
+        <v>739</v>
+      </c>
+      <c r="C7" t="s">
+        <v>808</v>
+      </c>
+      <c r="D7" t="s">
+        <v>820</v>
+      </c>
+      <c r="E7" t="s">
+        <v>832</v>
+      </c>
+      <c r="F7" t="s">
+        <v>845</v>
+      </c>
+      <c r="G7" t="s">
+        <v>858</v>
+      </c>
+      <c r="H7" t="s">
+        <v>869</v>
+      </c>
+      <c r="I7" t="s">
+        <v>879</v>
+      </c>
+      <c r="J7" t="s">
+        <v>890</v>
+      </c>
+      <c r="K7" t="s">
+        <v>903</v>
+      </c>
+      <c r="L7" t="s">
+        <v>909</v>
+      </c>
+      <c r="M7" t="s">
+        <v>917</v>
+      </c>
+      <c r="N7" t="s">
+        <v>928</v>
+      </c>
+      <c r="O7" t="s">
+        <v>935</v>
+      </c>
+    </row>
+    <row r="8" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A8" t="s">
+        <v>775</v>
+      </c>
+      <c r="B8" t="s">
+        <v>795</v>
+      </c>
+      <c r="C8" t="s">
+        <v>809</v>
+      </c>
+      <c r="D8" t="s">
+        <v>821</v>
+      </c>
+      <c r="E8" t="s">
+        <v>833</v>
+      </c>
+      <c r="F8" t="s">
+        <v>846</v>
+      </c>
+      <c r="G8" t="s">
+        <v>859</v>
+      </c>
+      <c r="H8" t="s">
+        <v>870</v>
+      </c>
+      <c r="I8" t="s">
+        <v>880</v>
+      </c>
+      <c r="J8" t="s">
+        <v>891</v>
+      </c>
+      <c r="K8" t="s">
+        <v>895</v>
+      </c>
+      <c r="L8" t="s">
+        <v>910</v>
+      </c>
+      <c r="M8" t="s">
+        <v>918</v>
+      </c>
+      <c r="O8" t="s">
+        <v>936</v>
+      </c>
+    </row>
+    <row r="9" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A9" t="s">
+        <v>785</v>
+      </c>
+      <c r="B9" t="s">
+        <v>796</v>
+      </c>
+      <c r="C9" t="s">
+        <v>810</v>
+      </c>
+      <c r="D9" t="s">
+        <v>822</v>
+      </c>
+      <c r="E9" t="s">
+        <v>834</v>
+      </c>
+      <c r="F9" t="s">
+        <v>847</v>
+      </c>
+      <c r="G9" t="s">
+        <v>860</v>
+      </c>
+      <c r="H9" t="s">
+        <v>871</v>
+      </c>
+      <c r="I9" t="s">
+        <v>881</v>
+      </c>
+      <c r="J9" t="s">
+        <v>892</v>
+      </c>
+      <c r="K9" t="s">
+        <v>896</v>
+      </c>
+      <c r="L9" t="s">
+        <v>911</v>
+      </c>
+      <c r="M9" t="s">
+        <v>919</v>
+      </c>
+    </row>
+    <row r="10" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A10" t="s">
+        <v>786</v>
+      </c>
+      <c r="B10" t="s">
+        <v>797</v>
+      </c>
+      <c r="C10" t="s">
+        <v>811</v>
+      </c>
+      <c r="D10" t="s">
+        <v>823</v>
+      </c>
+      <c r="E10" t="s">
+        <v>835</v>
+      </c>
+      <c r="F10" t="s">
+        <v>848</v>
+      </c>
+      <c r="G10" t="s">
+        <v>694</v>
+      </c>
+      <c r="H10" t="s">
+        <v>872</v>
+      </c>
+      <c r="I10" t="s">
+        <v>882</v>
+      </c>
+      <c r="K10" t="s">
+        <v>897</v>
+      </c>
+      <c r="M10" t="s">
+        <v>920</v>
+      </c>
+    </row>
+    <row r="11" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A11" t="s">
+        <v>787</v>
+      </c>
+      <c r="B11" t="s">
+        <v>798</v>
+      </c>
+      <c r="C11" t="s">
+        <v>812</v>
+      </c>
+      <c r="D11" t="s">
+        <v>824</v>
+      </c>
+      <c r="E11" t="s">
+        <v>836</v>
+      </c>
+      <c r="F11" t="s">
+        <v>849</v>
+      </c>
+      <c r="G11" t="s">
+        <v>861</v>
+      </c>
+      <c r="I11" t="s">
+        <v>883</v>
+      </c>
+      <c r="K11" t="s">
+        <v>898</v>
+      </c>
+      <c r="M11" t="s">
+        <v>921</v>
+      </c>
+    </row>
+    <row r="12" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A12" t="s">
+        <v>788</v>
+      </c>
+      <c r="B12" t="s">
+        <v>799</v>
+      </c>
+      <c r="C12" t="s">
+        <v>813</v>
+      </c>
+      <c r="D12" t="s">
+        <v>825</v>
+      </c>
+      <c r="E12" t="s">
+        <v>837</v>
+      </c>
+      <c r="F12" t="s">
+        <v>850</v>
+      </c>
+      <c r="G12" t="s">
+        <v>862</v>
+      </c>
+    </row>
+    <row r="13" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="B13" t="s">
+        <v>800</v>
+      </c>
+      <c r="C13" t="s">
+        <v>814</v>
+      </c>
+      <c r="D13" t="s">
+        <v>826</v>
+      </c>
+      <c r="E13" t="s">
+        <v>838</v>
+      </c>
+      <c r="F13" t="s">
+        <v>851</v>
+      </c>
+      <c r="G13" t="s">
+        <v>863</v>
+      </c>
+    </row>
+    <row r="14" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="B14" t="s">
+        <v>801</v>
+      </c>
+      <c r="C14" t="s">
+        <v>815</v>
+      </c>
+      <c r="E14" t="s">
+        <v>839</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ED26D502-4BF9-495F-B9B9-D5F463473EBE}">
+  <dimension ref="A1:T21"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="O31" sqref="O31"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetData>
+    <row r="1" spans="1:20" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
+        <v>937</v>
+      </c>
+      <c r="B1" t="s">
+        <v>950</v>
+      </c>
+      <c r="C1" t="s">
+        <v>966</v>
+      </c>
+      <c r="D1" t="s">
+        <v>983</v>
+      </c>
+      <c r="E1" t="s">
+        <v>999</v>
+      </c>
+      <c r="F1" t="s">
+        <v>318</v>
+      </c>
+      <c r="G1" t="s">
+        <v>1026</v>
+      </c>
+      <c r="H1" t="s">
+        <v>986</v>
+      </c>
+      <c r="I1" t="s">
+        <v>1052</v>
+      </c>
+      <c r="J1" t="s">
+        <v>1064</v>
+      </c>
+      <c r="K1" t="s">
+        <v>1078</v>
+      </c>
+      <c r="L1" t="s">
+        <v>1095</v>
+      </c>
+      <c r="M1" t="s">
+        <v>1108</v>
+      </c>
+      <c r="N1" t="s">
+        <v>1121</v>
+      </c>
+      <c r="O1" t="s">
+        <v>1137</v>
+      </c>
+      <c r="P1" t="s">
+        <v>1154</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>1166</v>
+      </c>
+      <c r="R1" t="s">
+        <v>1180</v>
+      </c>
+      <c r="S1" t="s">
+        <v>1196</v>
+      </c>
+      <c r="T1" t="s">
+        <v>1208</v>
+      </c>
+    </row>
+    <row r="2" spans="1:20" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>938</v>
+      </c>
+      <c r="B2" t="s">
+        <v>951</v>
+      </c>
+      <c r="C2" t="s">
+        <v>967</v>
+      </c>
+      <c r="D2" t="s">
+        <v>984</v>
+      </c>
+      <c r="E2" t="s">
+        <v>1000</v>
+      </c>
+      <c r="F2" t="s">
+        <v>1013</v>
+      </c>
+      <c r="G2" t="s">
+        <v>1027</v>
+      </c>
+      <c r="H2" t="s">
+        <v>1036</v>
+      </c>
+      <c r="I2" t="s">
+        <v>916</v>
+      </c>
+      <c r="J2" t="s">
+        <v>1065</v>
+      </c>
+      <c r="K2" t="s">
+        <v>1079</v>
+      </c>
+      <c r="L2" t="s">
+        <v>892</v>
+      </c>
+      <c r="M2" t="s">
+        <v>1109</v>
+      </c>
+      <c r="N2" t="s">
+        <v>1122</v>
+      </c>
+      <c r="O2" t="s">
+        <v>1138</v>
+      </c>
+      <c r="P2" t="s">
+        <v>1155</v>
+      </c>
+      <c r="Q2" t="s">
+        <v>1167</v>
+      </c>
+      <c r="R2" t="s">
+        <v>1181</v>
+      </c>
+      <c r="S2" t="s">
+        <v>1197</v>
+      </c>
+      <c r="T2" t="s">
+        <v>1209</v>
+      </c>
+    </row>
+    <row r="3" spans="1:20" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>766</v>
+      </c>
+      <c r="B3" t="s">
+        <v>952</v>
+      </c>
+      <c r="C3" t="s">
+        <v>968</v>
+      </c>
+      <c r="D3" t="s">
+        <v>985</v>
+      </c>
+      <c r="E3" t="s">
+        <v>1001</v>
+      </c>
+      <c r="F3" t="s">
+        <v>1014</v>
+      </c>
+      <c r="G3" t="s">
+        <v>1028</v>
+      </c>
+      <c r="H3" t="s">
+        <v>1037</v>
+      </c>
+      <c r="I3" t="s">
+        <v>1053</v>
+      </c>
+      <c r="J3" t="s">
+        <v>1066</v>
+      </c>
+      <c r="K3" t="s">
+        <v>1080</v>
+      </c>
+      <c r="L3" t="s">
+        <v>1096</v>
+      </c>
+      <c r="M3" t="s">
+        <v>1110</v>
+      </c>
+      <c r="N3" t="s">
+        <v>1123</v>
+      </c>
+      <c r="O3" t="s">
+        <v>1139</v>
+      </c>
+      <c r="P3" t="s">
+        <v>1156</v>
+      </c>
+      <c r="Q3" t="s">
+        <v>1168</v>
+      </c>
+      <c r="R3" t="s">
+        <v>976</v>
+      </c>
+      <c r="S3" t="s">
+        <v>1198</v>
+      </c>
+      <c r="T3" t="s">
+        <v>1210</v>
+      </c>
+    </row>
+    <row r="4" spans="1:20" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>939</v>
+      </c>
+      <c r="B4" t="s">
+        <v>953</v>
+      </c>
+      <c r="C4" t="s">
+        <v>969</v>
+      </c>
+      <c r="D4" t="s">
+        <v>986</v>
+      </c>
+      <c r="E4" t="s">
+        <v>1002</v>
+      </c>
+      <c r="F4" t="s">
+        <v>1015</v>
+      </c>
+      <c r="G4" t="s">
+        <v>1029</v>
+      </c>
+      <c r="H4" t="s">
+        <v>1038</v>
+      </c>
+      <c r="I4" t="s">
+        <v>1054</v>
+      </c>
+      <c r="J4" t="s">
+        <v>1067</v>
+      </c>
+      <c r="K4" t="s">
+        <v>832</v>
+      </c>
+      <c r="L4" t="s">
+        <v>1097</v>
+      </c>
+      <c r="M4" t="s">
+        <v>1111</v>
+      </c>
+      <c r="N4" t="s">
+        <v>1124</v>
+      </c>
+      <c r="O4" t="s">
+        <v>1140</v>
+      </c>
+      <c r="P4" t="s">
+        <v>1157</v>
+      </c>
+      <c r="Q4" t="s">
+        <v>1169</v>
+      </c>
+      <c r="R4" t="s">
+        <v>1182</v>
+      </c>
+      <c r="S4" t="s">
+        <v>1199</v>
+      </c>
+      <c r="T4" t="s">
+        <v>1211</v>
+      </c>
+    </row>
+    <row r="5" spans="1:20" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>919</v>
+      </c>
+      <c r="B5" t="s">
+        <v>954</v>
+      </c>
+      <c r="C5" t="s">
+        <v>970</v>
+      </c>
+      <c r="D5" t="s">
+        <v>987</v>
+      </c>
+      <c r="E5" t="s">
+        <v>1003</v>
+      </c>
+      <c r="F5" t="s">
+        <v>1016</v>
+      </c>
+      <c r="G5" t="s">
+        <v>1030</v>
+      </c>
+      <c r="H5" t="s">
+        <v>1039</v>
+      </c>
+      <c r="I5" t="s">
+        <v>1055</v>
+      </c>
+      <c r="J5" t="s">
+        <v>1068</v>
+      </c>
+      <c r="K5" t="s">
+        <v>1081</v>
+      </c>
+      <c r="L5" t="s">
+        <v>1098</v>
+      </c>
+      <c r="M5" t="s">
+        <v>1112</v>
+      </c>
+      <c r="N5" t="s">
+        <v>1125</v>
+      </c>
+      <c r="O5" t="s">
+        <v>1141</v>
+      </c>
+      <c r="P5" t="s">
+        <v>1158</v>
+      </c>
+      <c r="Q5" t="s">
+        <v>1170</v>
+      </c>
+      <c r="R5" t="s">
+        <v>1183</v>
+      </c>
+      <c r="S5" t="s">
+        <v>1004</v>
+      </c>
+      <c r="T5" t="s">
+        <v>1212</v>
+      </c>
+    </row>
+    <row r="6" spans="1:20" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
+        <v>940</v>
+      </c>
+      <c r="B6" t="s">
+        <v>955</v>
+      </c>
+      <c r="C6" t="s">
+        <v>971</v>
+      </c>
+      <c r="D6" t="s">
+        <v>988</v>
+      </c>
+      <c r="E6" t="s">
+        <v>1005</v>
+      </c>
+      <c r="F6" t="s">
+        <v>1017</v>
+      </c>
+      <c r="G6" t="s">
+        <v>1031</v>
+      </c>
+      <c r="H6" t="s">
+        <v>1040</v>
+      </c>
+      <c r="I6" t="s">
+        <v>1056</v>
+      </c>
+      <c r="J6" t="s">
+        <v>1069</v>
+      </c>
+      <c r="K6" t="s">
+        <v>1082</v>
+      </c>
+      <c r="L6" t="s">
+        <v>1099</v>
+      </c>
+      <c r="M6" t="s">
+        <v>1113</v>
+      </c>
+      <c r="N6" t="s">
+        <v>1126</v>
+      </c>
+      <c r="O6" t="s">
+        <v>1142</v>
+      </c>
+      <c r="P6" t="s">
+        <v>823</v>
+      </c>
+      <c r="Q6" t="s">
+        <v>1171</v>
+      </c>
+      <c r="R6" t="s">
+        <v>1184</v>
+      </c>
+      <c r="S6" t="s">
+        <v>1200</v>
+      </c>
+      <c r="T6" t="s">
+        <v>1213</v>
+      </c>
+    </row>
+    <row r="7" spans="1:20" x14ac:dyDescent="0.35">
+      <c r="A7" t="s">
+        <v>941</v>
+      </c>
+      <c r="B7" t="s">
+        <v>956</v>
+      </c>
+      <c r="C7" t="s">
+        <v>972</v>
+      </c>
+      <c r="D7" t="s">
+        <v>989</v>
+      </c>
+      <c r="E7" t="s">
+        <v>1006</v>
+      </c>
+      <c r="F7" t="s">
+        <v>1018</v>
+      </c>
+      <c r="G7" t="s">
+        <v>879</v>
+      </c>
+      <c r="H7" t="s">
+        <v>1041</v>
+      </c>
+      <c r="I7" t="s">
+        <v>1057</v>
+      </c>
+      <c r="J7" t="s">
+        <v>842</v>
+      </c>
+      <c r="K7" t="s">
+        <v>1083</v>
+      </c>
+      <c r="L7" t="s">
+        <v>1100</v>
+      </c>
+      <c r="M7" t="s">
+        <v>1114</v>
+      </c>
+      <c r="N7" t="s">
+        <v>1127</v>
+      </c>
+      <c r="O7" t="s">
+        <v>1143</v>
+      </c>
+      <c r="P7" t="s">
+        <v>1159</v>
+      </c>
+      <c r="Q7" t="s">
+        <v>1172</v>
+      </c>
+      <c r="R7" t="s">
+        <v>1185</v>
+      </c>
+      <c r="S7" t="s">
+        <v>1201</v>
+      </c>
+      <c r="T7" t="s">
+        <v>1214</v>
+      </c>
+    </row>
+    <row r="8" spans="1:20" x14ac:dyDescent="0.35">
+      <c r="A8" t="s">
+        <v>942</v>
+      </c>
+      <c r="B8" t="s">
+        <v>957</v>
+      </c>
+      <c r="C8" t="s">
+        <v>973</v>
+      </c>
+      <c r="D8" t="s">
+        <v>990</v>
+      </c>
+      <c r="E8" t="s">
+        <v>1007</v>
+      </c>
+      <c r="F8" t="s">
+        <v>1019</v>
+      </c>
+      <c r="G8" t="s">
+        <v>1032</v>
+      </c>
+      <c r="H8" t="s">
+        <v>1042</v>
+      </c>
+      <c r="I8" t="s">
+        <v>1058</v>
+      </c>
+      <c r="J8" t="s">
+        <v>1070</v>
+      </c>
+      <c r="K8" t="s">
+        <v>1084</v>
+      </c>
+      <c r="L8" t="s">
+        <v>1101</v>
+      </c>
+      <c r="M8" t="s">
+        <v>1115</v>
+      </c>
+      <c r="N8" t="s">
+        <v>681</v>
+      </c>
+      <c r="O8" t="s">
+        <v>1144</v>
+      </c>
+      <c r="P8" t="s">
+        <v>797</v>
+      </c>
+      <c r="Q8" t="s">
+        <v>1173</v>
+      </c>
+      <c r="R8" t="s">
+        <v>1186</v>
+      </c>
+      <c r="S8" t="s">
+        <v>1202</v>
+      </c>
+      <c r="T8" t="s">
+        <v>1215</v>
+      </c>
+    </row>
+    <row r="9" spans="1:20" x14ac:dyDescent="0.35">
+      <c r="A9" t="s">
+        <v>943</v>
+      </c>
+      <c r="B9" t="s">
+        <v>528</v>
+      </c>
+      <c r="C9" t="s">
+        <v>974</v>
+      </c>
+      <c r="D9" t="s">
+        <v>991</v>
+      </c>
+      <c r="E9" t="s">
+        <v>1008</v>
+      </c>
+      <c r="F9" t="s">
+        <v>1020</v>
+      </c>
+      <c r="G9" t="s">
+        <v>1033</v>
+      </c>
+      <c r="H9" t="s">
+        <v>1043</v>
+      </c>
+      <c r="I9" t="s">
+        <v>1059</v>
+      </c>
+      <c r="J9" t="s">
+        <v>1071</v>
+      </c>
+      <c r="K9" t="s">
+        <v>1085</v>
+      </c>
+      <c r="L9" t="s">
+        <v>1102</v>
+      </c>
+      <c r="M9" t="s">
+        <v>1116</v>
+      </c>
+      <c r="N9" t="s">
+        <v>1128</v>
+      </c>
+      <c r="O9" t="s">
+        <v>1145</v>
+      </c>
+      <c r="P9" t="s">
+        <v>850</v>
+      </c>
+      <c r="Q9" t="s">
+        <v>1174</v>
+      </c>
+      <c r="R9" t="s">
+        <v>1187</v>
+      </c>
+      <c r="S9" t="s">
+        <v>861</v>
+      </c>
+      <c r="T9" t="s">
+        <v>1216</v>
+      </c>
+    </row>
+    <row r="10" spans="1:20" x14ac:dyDescent="0.35">
+      <c r="A10" t="s">
+        <v>944</v>
+      </c>
+      <c r="B10" t="s">
+        <v>958</v>
+      </c>
+      <c r="C10" t="s">
+        <v>975</v>
+      </c>
+      <c r="D10" t="s">
+        <v>992</v>
+      </c>
+      <c r="E10" t="s">
+        <v>1009</v>
+      </c>
+      <c r="F10" t="s">
+        <v>1021</v>
+      </c>
+      <c r="G10" t="s">
+        <v>818</v>
+      </c>
+      <c r="H10" t="s">
+        <v>1044</v>
+      </c>
+      <c r="I10" t="s">
+        <v>1060</v>
+      </c>
+      <c r="J10" t="s">
+        <v>1072</v>
+      </c>
+      <c r="K10" t="s">
+        <v>1086</v>
+      </c>
+      <c r="L10" t="s">
+        <v>1103</v>
+      </c>
+      <c r="M10" t="s">
+        <v>1117</v>
+      </c>
+      <c r="N10" t="s">
+        <v>1129</v>
+      </c>
+      <c r="O10" t="s">
+        <v>108</v>
+      </c>
+      <c r="P10" t="s">
+        <v>1160</v>
+      </c>
+      <c r="Q10" t="s">
+        <v>1175</v>
+      </c>
+      <c r="R10" t="s">
+        <v>1188</v>
+      </c>
+      <c r="S10" t="s">
+        <v>1203</v>
+      </c>
+      <c r="T10" t="s">
+        <v>1217</v>
+      </c>
+    </row>
+    <row r="11" spans="1:20" x14ac:dyDescent="0.35">
+      <c r="A11" t="s">
+        <v>945</v>
+      </c>
+      <c r="B11" t="s">
+        <v>959</v>
+      </c>
+      <c r="C11" t="s">
+        <v>976</v>
+      </c>
+      <c r="D11" t="s">
+        <v>993</v>
+      </c>
+      <c r="E11" t="s">
+        <v>1010</v>
+      </c>
+      <c r="F11" t="s">
+        <v>1022</v>
+      </c>
+      <c r="G11" t="s">
+        <v>1034</v>
+      </c>
+      <c r="H11" t="s">
+        <v>1045</v>
+      </c>
+      <c r="I11" t="s">
+        <v>1061</v>
+      </c>
+      <c r="J11" t="s">
+        <v>1073</v>
+      </c>
+      <c r="K11" t="s">
+        <v>1087</v>
+      </c>
+      <c r="L11" t="s">
+        <v>1104</v>
+      </c>
+      <c r="M11" t="s">
+        <v>1118</v>
+      </c>
+      <c r="N11" t="s">
+        <v>1130</v>
+      </c>
+      <c r="O11" t="s">
+        <v>1152</v>
+      </c>
+      <c r="P11" t="s">
+        <v>1161</v>
+      </c>
+      <c r="Q11" t="s">
+        <v>1176</v>
+      </c>
+      <c r="R11" t="s">
+        <v>1189</v>
+      </c>
+      <c r="S11" t="s">
+        <v>1204</v>
+      </c>
+      <c r="T11" t="s">
+        <v>722</v>
+      </c>
+    </row>
+    <row r="12" spans="1:20" x14ac:dyDescent="0.35">
+      <c r="A12" t="s">
+        <v>946</v>
+      </c>
+      <c r="B12" t="s">
+        <v>960</v>
+      </c>
+      <c r="C12" t="s">
+        <v>977</v>
+      </c>
+      <c r="D12" t="s">
+        <v>994</v>
+      </c>
+      <c r="E12" t="s">
+        <v>1011</v>
+      </c>
+      <c r="F12" t="s">
+        <v>1023</v>
+      </c>
+      <c r="G12" t="s">
+        <v>1035</v>
+      </c>
+      <c r="H12" t="s">
+        <v>1046</v>
+      </c>
+      <c r="I12" t="s">
+        <v>1062</v>
+      </c>
+      <c r="J12" t="s">
+        <v>1074</v>
+      </c>
+      <c r="K12" t="s">
+        <v>1088</v>
+      </c>
+      <c r="L12" t="s">
+        <v>1105</v>
+      </c>
+      <c r="M12" t="s">
+        <v>260</v>
+      </c>
+      <c r="N12" t="s">
+        <v>1131</v>
+      </c>
+      <c r="O12" t="s">
+        <v>1146</v>
+      </c>
+      <c r="P12" t="s">
+        <v>1162</v>
+      </c>
+      <c r="Q12" t="s">
+        <v>1177</v>
+      </c>
+      <c r="R12" t="s">
+        <v>1190</v>
+      </c>
+      <c r="S12" t="s">
+        <v>1205</v>
+      </c>
+      <c r="T12" t="s">
+        <v>1218</v>
+      </c>
+    </row>
+    <row r="13" spans="1:20" x14ac:dyDescent="0.35">
+      <c r="A13" t="s">
+        <v>947</v>
+      </c>
+      <c r="B13" t="s">
+        <v>914</v>
+      </c>
+      <c r="C13" t="s">
+        <v>978</v>
+      </c>
+      <c r="D13" t="s">
+        <v>995</v>
+      </c>
+      <c r="E13" t="s">
+        <v>1012</v>
+      </c>
+      <c r="F13" t="s">
+        <v>1024</v>
+      </c>
+      <c r="H13" t="s">
+        <v>1047</v>
+      </c>
+      <c r="I13" t="s">
+        <v>1063</v>
+      </c>
+      <c r="J13" t="s">
+        <v>1075</v>
+      </c>
+      <c r="K13" t="s">
+        <v>1089</v>
+      </c>
+      <c r="L13" t="s">
+        <v>1106</v>
+      </c>
+      <c r="M13" t="s">
+        <v>1119</v>
+      </c>
+      <c r="N13" t="s">
+        <v>1132</v>
+      </c>
+      <c r="O13" t="s">
+        <v>1147</v>
+      </c>
+      <c r="P13" t="s">
+        <v>1163</v>
+      </c>
+      <c r="Q13" t="s">
+        <v>1178</v>
+      </c>
+      <c r="R13" t="s">
+        <v>1191</v>
+      </c>
+      <c r="S13" t="s">
+        <v>1206</v>
+      </c>
+      <c r="T13" t="s">
+        <v>1219</v>
+      </c>
+    </row>
+    <row r="14" spans="1:20" x14ac:dyDescent="0.35">
+      <c r="A14" t="s">
+        <v>948</v>
+      </c>
+      <c r="B14" t="s">
+        <v>961</v>
+      </c>
+      <c r="C14" t="s">
+        <v>979</v>
+      </c>
+      <c r="D14" t="s">
+        <v>996</v>
+      </c>
+      <c r="F14" t="s">
+        <v>1025</v>
+      </c>
+      <c r="H14" t="s">
+        <v>1048</v>
+      </c>
+      <c r="J14" t="s">
+        <v>1076</v>
+      </c>
+      <c r="K14" t="s">
+        <v>1090</v>
+      </c>
+      <c r="L14" t="s">
+        <v>1107</v>
+      </c>
+      <c r="M14" t="s">
+        <v>1120</v>
+      </c>
+      <c r="N14" t="s">
+        <v>1133</v>
+      </c>
+      <c r="O14" t="s">
+        <v>981</v>
+      </c>
+      <c r="P14" t="s">
+        <v>1164</v>
+      </c>
+      <c r="Q14" t="s">
+        <v>525</v>
+      </c>
+      <c r="R14" t="s">
+        <v>1192</v>
+      </c>
+      <c r="S14" t="s">
+        <v>1207</v>
+      </c>
+      <c r="T14" t="s">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="15" spans="1:20" x14ac:dyDescent="0.35">
+      <c r="A15" t="s">
+        <v>949</v>
+      </c>
+      <c r="B15" t="s">
+        <v>962</v>
+      </c>
+      <c r="C15" t="s">
+        <v>980</v>
+      </c>
+      <c r="D15" t="s">
+        <v>997</v>
+      </c>
+      <c r="F15" t="s">
+        <v>934</v>
+      </c>
+      <c r="H15" t="s">
+        <v>1049</v>
+      </c>
+      <c r="J15" t="s">
+        <v>1077</v>
+      </c>
+      <c r="K15" t="s">
+        <v>649</v>
+      </c>
+      <c r="M15" t="s">
+        <v>849</v>
+      </c>
+      <c r="N15" t="s">
+        <v>1134</v>
+      </c>
+      <c r="O15" t="s">
+        <v>1148</v>
+      </c>
+      <c r="P15" t="s">
+        <v>1165</v>
+      </c>
+      <c r="Q15" t="s">
+        <v>649</v>
+      </c>
+      <c r="R15" t="s">
+        <v>1193</v>
+      </c>
+      <c r="T15" t="s">
+        <v>1220</v>
+      </c>
+    </row>
+    <row r="16" spans="1:20" x14ac:dyDescent="0.35">
+      <c r="B16" t="s">
+        <v>963</v>
+      </c>
+      <c r="C16" t="s">
+        <v>981</v>
+      </c>
+      <c r="D16" t="s">
+        <v>998</v>
+      </c>
+      <c r="H16" t="s">
+        <v>1050</v>
+      </c>
+      <c r="K16" t="s">
+        <v>1091</v>
+      </c>
+      <c r="N16" t="s">
+        <v>1135</v>
+      </c>
+      <c r="O16" t="s">
+        <v>1149</v>
+      </c>
+      <c r="P16" t="s">
+        <v>90</v>
+      </c>
+      <c r="Q16" t="s">
+        <v>1179</v>
+      </c>
+      <c r="R16" t="s">
+        <v>566</v>
+      </c>
+    </row>
+    <row r="17" spans="2:18" x14ac:dyDescent="0.35">
+      <c r="B17" t="s">
+        <v>964</v>
+      </c>
+      <c r="C17" t="s">
+        <v>982</v>
+      </c>
+      <c r="H17" t="s">
+        <v>1051</v>
+      </c>
+      <c r="K17" t="s">
+        <v>1092</v>
+      </c>
+      <c r="N17" t="s">
+        <v>1136</v>
+      </c>
+      <c r="O17" t="s">
+        <v>385</v>
+      </c>
+      <c r="R17" t="s">
+        <v>1194</v>
+      </c>
+    </row>
+    <row r="18" spans="2:18" x14ac:dyDescent="0.35">
+      <c r="B18" t="s">
+        <v>965</v>
+      </c>
+      <c r="K18" t="s">
+        <v>1093</v>
+      </c>
+      <c r="O18" t="s">
+        <v>1150</v>
+      </c>
+      <c r="R18" t="s">
+        <v>1195</v>
+      </c>
+    </row>
+    <row r="19" spans="2:18" x14ac:dyDescent="0.35">
+      <c r="K19" t="s">
+        <v>1094</v>
+      </c>
+      <c r="O19" t="s">
+        <v>1151</v>
+      </c>
+    </row>
+    <row r="20" spans="2:18" x14ac:dyDescent="0.35">
+      <c r="O20" t="s">
+        <v>584</v>
+      </c>
+    </row>
+    <row r="21" spans="2:18" x14ac:dyDescent="0.35">
+      <c r="O21" t="s">
+        <v>1153</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:T33"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="Q10" sqref="Q10"/>
     </sheetView>
   </sheetViews>

</xml_diff>